<commit_message>
deleting all code, because will be fully updated
</commit_message>
<xml_diff>
--- a/_data/ADAUSDT_1h.xlsx
+++ b/_data/ADAUSDT_1h.xlsx
@@ -395,7 +395,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F1335"/>
+  <dimension ref="A1:F1464"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -27101,6 +27101,2586 @@
         <v>975307.3</v>
       </c>
     </row>
+    <row r="1336" spans="1:6">
+      <c r="A1336" s="2">
+        <v>45534.45833333334</v>
+      </c>
+      <c r="B1336">
+        <v>0.3582</v>
+      </c>
+      <c r="C1336">
+        <v>0.3587</v>
+      </c>
+      <c r="D1336">
+        <v>0.3508</v>
+      </c>
+      <c r="E1336">
+        <v>0.3513</v>
+      </c>
+      <c r="F1336">
+        <v>11386486.6</v>
+      </c>
+    </row>
+    <row r="1337" spans="1:6">
+      <c r="A1337" s="2">
+        <v>45534.5</v>
+      </c>
+      <c r="B1337">
+        <v>0.3513</v>
+      </c>
+      <c r="C1337">
+        <v>0.3546</v>
+      </c>
+      <c r="D1337">
+        <v>0.349</v>
+      </c>
+      <c r="E1337">
+        <v>0.35</v>
+      </c>
+      <c r="F1337">
+        <v>16007397.3</v>
+      </c>
+    </row>
+    <row r="1338" spans="1:6">
+      <c r="A1338" s="2">
+        <v>45534.54166666666</v>
+      </c>
+      <c r="B1338">
+        <v>0.35</v>
+      </c>
+      <c r="C1338">
+        <v>0.3522</v>
+      </c>
+      <c r="D1338">
+        <v>0.3461</v>
+      </c>
+      <c r="E1338">
+        <v>0.3519</v>
+      </c>
+      <c r="F1338">
+        <v>8325666.4</v>
+      </c>
+    </row>
+    <row r="1339" spans="1:6">
+      <c r="A1339" s="2">
+        <v>45534.58333333334</v>
+      </c>
+      <c r="B1339">
+        <v>0.352</v>
+      </c>
+      <c r="C1339">
+        <v>0.3543</v>
+      </c>
+      <c r="D1339">
+        <v>0.3445</v>
+      </c>
+      <c r="E1339">
+        <v>0.3445</v>
+      </c>
+      <c r="F1339">
+        <v>8053687.5</v>
+      </c>
+    </row>
+    <row r="1340" spans="1:6">
+      <c r="A1340" s="2">
+        <v>45534.625</v>
+      </c>
+      <c r="B1340">
+        <v>0.3446</v>
+      </c>
+      <c r="C1340">
+        <v>0.3458</v>
+      </c>
+      <c r="D1340">
+        <v>0.3383</v>
+      </c>
+      <c r="E1340">
+        <v>0.34</v>
+      </c>
+      <c r="F1340">
+        <v>15454758</v>
+      </c>
+    </row>
+    <row r="1341" spans="1:6">
+      <c r="A1341" s="2">
+        <v>45534.66666666666</v>
+      </c>
+      <c r="B1341">
+        <v>0.34</v>
+      </c>
+      <c r="C1341">
+        <v>0.3432</v>
+      </c>
+      <c r="D1341">
+        <v>0.3373</v>
+      </c>
+      <c r="E1341">
+        <v>0.3428</v>
+      </c>
+      <c r="F1341">
+        <v>7675247.9</v>
+      </c>
+    </row>
+    <row r="1342" spans="1:6">
+      <c r="A1342" s="2">
+        <v>45534.70833333334</v>
+      </c>
+      <c r="B1342">
+        <v>0.3428</v>
+      </c>
+      <c r="C1342">
+        <v>0.3436</v>
+      </c>
+      <c r="D1342">
+        <v>0.3415</v>
+      </c>
+      <c r="E1342">
+        <v>0.343</v>
+      </c>
+      <c r="F1342">
+        <v>2974953.6</v>
+      </c>
+    </row>
+    <row r="1343" spans="1:6">
+      <c r="A1343" s="2">
+        <v>45534.75</v>
+      </c>
+      <c r="B1343">
+        <v>0.3429</v>
+      </c>
+      <c r="C1343">
+        <v>0.3493</v>
+      </c>
+      <c r="D1343">
+        <v>0.3426</v>
+      </c>
+      <c r="E1343">
+        <v>0.3487</v>
+      </c>
+      <c r="F1343">
+        <v>4224871.7</v>
+      </c>
+    </row>
+    <row r="1344" spans="1:6">
+      <c r="A1344" s="2">
+        <v>45534.79166666666</v>
+      </c>
+      <c r="B1344">
+        <v>0.3487</v>
+      </c>
+      <c r="C1344">
+        <v>0.3487</v>
+      </c>
+      <c r="D1344">
+        <v>0.3442</v>
+      </c>
+      <c r="E1344">
+        <v>0.3455</v>
+      </c>
+      <c r="F1344">
+        <v>1763338.4</v>
+      </c>
+    </row>
+    <row r="1345" spans="1:6">
+      <c r="A1345" s="2">
+        <v>45534.83333333334</v>
+      </c>
+      <c r="B1345">
+        <v>0.3455</v>
+      </c>
+      <c r="C1345">
+        <v>0.3476</v>
+      </c>
+      <c r="D1345">
+        <v>0.3455</v>
+      </c>
+      <c r="E1345">
+        <v>0.3471</v>
+      </c>
+      <c r="F1345">
+        <v>906200.1</v>
+      </c>
+    </row>
+    <row r="1346" spans="1:6">
+      <c r="A1346" s="2">
+        <v>45534.875</v>
+      </c>
+      <c r="B1346">
+        <v>0.3471</v>
+      </c>
+      <c r="C1346">
+        <v>0.3479</v>
+      </c>
+      <c r="D1346">
+        <v>0.3464</v>
+      </c>
+      <c r="E1346">
+        <v>0.3469</v>
+      </c>
+      <c r="F1346">
+        <v>940593.2</v>
+      </c>
+    </row>
+    <row r="1347" spans="1:6">
+      <c r="A1347" s="2">
+        <v>45534.91666666666</v>
+      </c>
+      <c r="B1347">
+        <v>0.3469</v>
+      </c>
+      <c r="C1347">
+        <v>0.348</v>
+      </c>
+      <c r="D1347">
+        <v>0.3465</v>
+      </c>
+      <c r="E1347">
+        <v>0.3476</v>
+      </c>
+      <c r="F1347">
+        <v>1521374.2</v>
+      </c>
+    </row>
+    <row r="1348" spans="1:6">
+      <c r="A1348" s="2">
+        <v>45534.95833333334</v>
+      </c>
+      <c r="B1348">
+        <v>0.3477</v>
+      </c>
+      <c r="C1348">
+        <v>0.3482</v>
+      </c>
+      <c r="D1348">
+        <v>0.3466</v>
+      </c>
+      <c r="E1348">
+        <v>0.3469</v>
+      </c>
+      <c r="F1348">
+        <v>1058132.6</v>
+      </c>
+    </row>
+    <row r="1349" spans="1:6">
+      <c r="A1349" s="2">
+        <v>45535</v>
+      </c>
+      <c r="B1349">
+        <v>0.3469</v>
+      </c>
+      <c r="C1349">
+        <v>0.3485</v>
+      </c>
+      <c r="D1349">
+        <v>0.3458</v>
+      </c>
+      <c r="E1349">
+        <v>0.3471</v>
+      </c>
+      <c r="F1349">
+        <v>1750537.7</v>
+      </c>
+    </row>
+    <row r="1350" spans="1:6">
+      <c r="A1350" s="2">
+        <v>45535.04166666666</v>
+      </c>
+      <c r="B1350">
+        <v>0.3472</v>
+      </c>
+      <c r="C1350">
+        <v>0.3473</v>
+      </c>
+      <c r="D1350">
+        <v>0.3467</v>
+      </c>
+      <c r="E1350">
+        <v>0.3469</v>
+      </c>
+      <c r="F1350">
+        <v>80490.7</v>
+      </c>
+    </row>
+    <row r="1351" spans="1:6">
+      <c r="A1351" s="2">
+        <v>45535.08333333334</v>
+      </c>
+      <c r="B1351">
+        <v>0.3467</v>
+      </c>
+      <c r="C1351">
+        <v>0.347</v>
+      </c>
+      <c r="D1351">
+        <v>0.346</v>
+      </c>
+      <c r="E1351">
+        <v>0.3463</v>
+      </c>
+      <c r="F1351">
+        <v>643760</v>
+      </c>
+    </row>
+    <row r="1352" spans="1:6">
+      <c r="A1352" s="2">
+        <v>45535.125</v>
+      </c>
+      <c r="B1352">
+        <v>0.3463</v>
+      </c>
+      <c r="C1352">
+        <v>0.3477</v>
+      </c>
+      <c r="D1352">
+        <v>0.3454</v>
+      </c>
+      <c r="E1352">
+        <v>0.3475</v>
+      </c>
+      <c r="F1352">
+        <v>1488614.7</v>
+      </c>
+    </row>
+    <row r="1353" spans="1:6">
+      <c r="A1353" s="2">
+        <v>45535.16666666666</v>
+      </c>
+      <c r="B1353">
+        <v>0.3474</v>
+      </c>
+      <c r="C1353">
+        <v>0.3504</v>
+      </c>
+      <c r="D1353">
+        <v>0.3474</v>
+      </c>
+      <c r="E1353">
+        <v>0.35</v>
+      </c>
+      <c r="F1353">
+        <v>1850475.3</v>
+      </c>
+    </row>
+    <row r="1354" spans="1:6">
+      <c r="A1354" s="2">
+        <v>45535.20833333334</v>
+      </c>
+      <c r="B1354">
+        <v>0.3499</v>
+      </c>
+      <c r="C1354">
+        <v>0.3502</v>
+      </c>
+      <c r="D1354">
+        <v>0.3479</v>
+      </c>
+      <c r="E1354">
+        <v>0.348</v>
+      </c>
+      <c r="F1354">
+        <v>812578.9</v>
+      </c>
+    </row>
+    <row r="1355" spans="1:6">
+      <c r="A1355" s="2">
+        <v>45535.25</v>
+      </c>
+      <c r="B1355">
+        <v>0.348</v>
+      </c>
+      <c r="C1355">
+        <v>0.3501</v>
+      </c>
+      <c r="D1355">
+        <v>0.3475</v>
+      </c>
+      <c r="E1355">
+        <v>0.3494</v>
+      </c>
+      <c r="F1355">
+        <v>1481570.9</v>
+      </c>
+    </row>
+    <row r="1356" spans="1:6">
+      <c r="A1356" s="2">
+        <v>45535.29166666666</v>
+      </c>
+      <c r="B1356">
+        <v>0.3494</v>
+      </c>
+      <c r="C1356">
+        <v>0.3496</v>
+      </c>
+      <c r="D1356">
+        <v>0.3478</v>
+      </c>
+      <c r="E1356">
+        <v>0.3478</v>
+      </c>
+      <c r="F1356">
+        <v>1017090.7</v>
+      </c>
+    </row>
+    <row r="1357" spans="1:6">
+      <c r="A1357" s="2">
+        <v>45535.33333333334</v>
+      </c>
+      <c r="B1357">
+        <v>0.3478</v>
+      </c>
+      <c r="C1357">
+        <v>0.3484</v>
+      </c>
+      <c r="D1357">
+        <v>0.3459</v>
+      </c>
+      <c r="E1357">
+        <v>0.346</v>
+      </c>
+      <c r="F1357">
+        <v>1068956</v>
+      </c>
+    </row>
+    <row r="1358" spans="1:6">
+      <c r="A1358" s="2">
+        <v>45535.375</v>
+      </c>
+      <c r="B1358">
+        <v>0.346</v>
+      </c>
+      <c r="C1358">
+        <v>0.3467</v>
+      </c>
+      <c r="D1358">
+        <v>0.3453</v>
+      </c>
+      <c r="E1358">
+        <v>0.3458</v>
+      </c>
+      <c r="F1358">
+        <v>1333364.6</v>
+      </c>
+    </row>
+    <row r="1359" spans="1:6">
+      <c r="A1359" s="2">
+        <v>45535.41666666666</v>
+      </c>
+      <c r="B1359">
+        <v>0.3458</v>
+      </c>
+      <c r="C1359">
+        <v>0.3483</v>
+      </c>
+      <c r="D1359">
+        <v>0.3454</v>
+      </c>
+      <c r="E1359">
+        <v>0.3476</v>
+      </c>
+      <c r="F1359">
+        <v>1625082.6</v>
+      </c>
+    </row>
+    <row r="1360" spans="1:6">
+      <c r="A1360" s="2">
+        <v>45535.45833333334</v>
+      </c>
+      <c r="B1360">
+        <v>0.3476</v>
+      </c>
+      <c r="C1360">
+        <v>0.3495</v>
+      </c>
+      <c r="D1360">
+        <v>0.3476</v>
+      </c>
+      <c r="E1360">
+        <v>0.3481</v>
+      </c>
+      <c r="F1360">
+        <v>782245.2</v>
+      </c>
+    </row>
+    <row r="1361" spans="1:6">
+      <c r="A1361" s="2">
+        <v>45535.5</v>
+      </c>
+      <c r="B1361">
+        <v>0.3481</v>
+      </c>
+      <c r="C1361">
+        <v>0.3488</v>
+      </c>
+      <c r="D1361">
+        <v>0.3475</v>
+      </c>
+      <c r="E1361">
+        <v>0.3482</v>
+      </c>
+      <c r="F1361">
+        <v>942067.8</v>
+      </c>
+    </row>
+    <row r="1362" spans="1:6">
+      <c r="A1362" s="2">
+        <v>45535.54166666666</v>
+      </c>
+      <c r="B1362">
+        <v>0.3481</v>
+      </c>
+      <c r="C1362">
+        <v>0.349</v>
+      </c>
+      <c r="D1362">
+        <v>0.3473</v>
+      </c>
+      <c r="E1362">
+        <v>0.3475</v>
+      </c>
+      <c r="F1362">
+        <v>1314650.6</v>
+      </c>
+    </row>
+    <row r="1363" spans="1:6">
+      <c r="A1363" s="2">
+        <v>45535.58333333334</v>
+      </c>
+      <c r="B1363">
+        <v>0.3475</v>
+      </c>
+      <c r="C1363">
+        <v>0.3484</v>
+      </c>
+      <c r="D1363">
+        <v>0.3471</v>
+      </c>
+      <c r="E1363">
+        <v>0.3484</v>
+      </c>
+      <c r="F1363">
+        <v>800958.4</v>
+      </c>
+    </row>
+    <row r="1364" spans="1:6">
+      <c r="A1364" s="2">
+        <v>45535.625</v>
+      </c>
+      <c r="B1364">
+        <v>0.3484</v>
+      </c>
+      <c r="C1364">
+        <v>0.3496</v>
+      </c>
+      <c r="D1364">
+        <v>0.3474</v>
+      </c>
+      <c r="E1364">
+        <v>0.3492</v>
+      </c>
+      <c r="F1364">
+        <v>1654453.9</v>
+      </c>
+    </row>
+    <row r="1365" spans="1:6">
+      <c r="A1365" s="2">
+        <v>45535.66666666666</v>
+      </c>
+      <c r="B1365">
+        <v>0.3492</v>
+      </c>
+      <c r="C1365">
+        <v>0.3493</v>
+      </c>
+      <c r="D1365">
+        <v>0.3473</v>
+      </c>
+      <c r="E1365">
+        <v>0.3481</v>
+      </c>
+      <c r="F1365">
+        <v>786501.1</v>
+      </c>
+    </row>
+    <row r="1366" spans="1:6">
+      <c r="A1366" s="2">
+        <v>45535.70833333334</v>
+      </c>
+      <c r="B1366">
+        <v>0.3481</v>
+      </c>
+      <c r="C1366">
+        <v>0.3491</v>
+      </c>
+      <c r="D1366">
+        <v>0.345</v>
+      </c>
+      <c r="E1366">
+        <v>0.3471</v>
+      </c>
+      <c r="F1366">
+        <v>1509847.6</v>
+      </c>
+    </row>
+    <row r="1367" spans="1:6">
+      <c r="A1367" s="2">
+        <v>45535.75</v>
+      </c>
+      <c r="B1367">
+        <v>0.3469</v>
+      </c>
+      <c r="C1367">
+        <v>0.3486</v>
+      </c>
+      <c r="D1367">
+        <v>0.3457</v>
+      </c>
+      <c r="E1367">
+        <v>0.3458</v>
+      </c>
+      <c r="F1367">
+        <v>1190894.5</v>
+      </c>
+    </row>
+    <row r="1368" spans="1:6">
+      <c r="A1368" s="2">
+        <v>45535.79166666666</v>
+      </c>
+      <c r="B1368">
+        <v>0.3458</v>
+      </c>
+      <c r="C1368">
+        <v>0.3469</v>
+      </c>
+      <c r="D1368">
+        <v>0.3455</v>
+      </c>
+      <c r="E1368">
+        <v>0.3468</v>
+      </c>
+      <c r="F1368">
+        <v>1264345.2</v>
+      </c>
+    </row>
+    <row r="1369" spans="1:6">
+      <c r="A1369" s="2">
+        <v>45535.83333333334</v>
+      </c>
+      <c r="B1369">
+        <v>0.3467</v>
+      </c>
+      <c r="C1369">
+        <v>0.347</v>
+      </c>
+      <c r="D1369">
+        <v>0.3458</v>
+      </c>
+      <c r="E1369">
+        <v>0.3458</v>
+      </c>
+      <c r="F1369">
+        <v>594099.3</v>
+      </c>
+    </row>
+    <row r="1370" spans="1:6">
+      <c r="A1370" s="2">
+        <v>45535.875</v>
+      </c>
+      <c r="B1370">
+        <v>0.3459</v>
+      </c>
+      <c r="C1370">
+        <v>0.346</v>
+      </c>
+      <c r="D1370">
+        <v>0.3447</v>
+      </c>
+      <c r="E1370">
+        <v>0.345</v>
+      </c>
+      <c r="F1370">
+        <v>550646.5</v>
+      </c>
+    </row>
+    <row r="1371" spans="1:6">
+      <c r="A1371" s="2">
+        <v>45535.91666666666</v>
+      </c>
+      <c r="B1371">
+        <v>0.3462</v>
+      </c>
+      <c r="C1371">
+        <v>0.3464</v>
+      </c>
+      <c r="D1371">
+        <v>0.3449</v>
+      </c>
+      <c r="E1371">
+        <v>0.3453</v>
+      </c>
+      <c r="F1371">
+        <v>780020.2</v>
+      </c>
+    </row>
+    <row r="1372" spans="1:6">
+      <c r="A1372" s="2">
+        <v>45535.95833333334</v>
+      </c>
+      <c r="B1372">
+        <v>0.3452</v>
+      </c>
+      <c r="C1372">
+        <v>0.3457</v>
+      </c>
+      <c r="D1372">
+        <v>0.3444</v>
+      </c>
+      <c r="E1372">
+        <v>0.345</v>
+      </c>
+      <c r="F1372">
+        <v>408066.1</v>
+      </c>
+    </row>
+    <row r="1373" spans="1:6">
+      <c r="A1373" s="2">
+        <v>45536</v>
+      </c>
+      <c r="B1373">
+        <v>0.3451</v>
+      </c>
+      <c r="C1373">
+        <v>0.3458</v>
+      </c>
+      <c r="D1373">
+        <v>0.3437</v>
+      </c>
+      <c r="E1373">
+        <v>0.3444</v>
+      </c>
+      <c r="F1373">
+        <v>1380857.6</v>
+      </c>
+    </row>
+    <row r="1374" spans="1:6">
+      <c r="A1374" s="2">
+        <v>45536.04166666666</v>
+      </c>
+      <c r="B1374">
+        <v>0.3443</v>
+      </c>
+      <c r="C1374">
+        <v>0.3445</v>
+      </c>
+      <c r="D1374">
+        <v>0.3413</v>
+      </c>
+      <c r="E1374">
+        <v>0.3414</v>
+      </c>
+      <c r="F1374">
+        <v>1403464.9</v>
+      </c>
+    </row>
+    <row r="1375" spans="1:6">
+      <c r="A1375" s="2">
+        <v>45536.08333333334</v>
+      </c>
+      <c r="B1375">
+        <v>0.3414</v>
+      </c>
+      <c r="C1375">
+        <v>0.3422</v>
+      </c>
+      <c r="D1375">
+        <v>0.3394</v>
+      </c>
+      <c r="E1375">
+        <v>0.3422</v>
+      </c>
+      <c r="F1375">
+        <v>2785916.1</v>
+      </c>
+    </row>
+    <row r="1376" spans="1:6">
+      <c r="A1376" s="2">
+        <v>45536.125</v>
+      </c>
+      <c r="B1376">
+        <v>0.3422</v>
+      </c>
+      <c r="C1376">
+        <v>0.3449</v>
+      </c>
+      <c r="D1376">
+        <v>0.3418</v>
+      </c>
+      <c r="E1376">
+        <v>0.3448</v>
+      </c>
+      <c r="F1376">
+        <v>832768.8</v>
+      </c>
+    </row>
+    <row r="1377" spans="1:6">
+      <c r="A1377" s="2">
+        <v>45536.16666666666</v>
+      </c>
+      <c r="B1377">
+        <v>0.3449</v>
+      </c>
+      <c r="C1377">
+        <v>0.3449</v>
+      </c>
+      <c r="D1377">
+        <v>0.3423</v>
+      </c>
+      <c r="E1377">
+        <v>0.3431</v>
+      </c>
+      <c r="F1377">
+        <v>1332148</v>
+      </c>
+    </row>
+    <row r="1378" spans="1:6">
+      <c r="A1378" s="2">
+        <v>45536.20833333334</v>
+      </c>
+      <c r="B1378">
+        <v>0.343</v>
+      </c>
+      <c r="C1378">
+        <v>0.3436</v>
+      </c>
+      <c r="D1378">
+        <v>0.3393</v>
+      </c>
+      <c r="E1378">
+        <v>0.3402</v>
+      </c>
+      <c r="F1378">
+        <v>2428889.6</v>
+      </c>
+    </row>
+    <row r="1379" spans="1:6">
+      <c r="A1379" s="2">
+        <v>45536.25</v>
+      </c>
+      <c r="B1379">
+        <v>0.3401</v>
+      </c>
+      <c r="C1379">
+        <v>0.3429</v>
+      </c>
+      <c r="D1379">
+        <v>0.34</v>
+      </c>
+      <c r="E1379">
+        <v>0.3427</v>
+      </c>
+      <c r="F1379">
+        <v>868632.2</v>
+      </c>
+    </row>
+    <row r="1380" spans="1:6">
+      <c r="A1380" s="2">
+        <v>45536.29166666666</v>
+      </c>
+      <c r="B1380">
+        <v>0.3427</v>
+      </c>
+      <c r="C1380">
+        <v>0.3446</v>
+      </c>
+      <c r="D1380">
+        <v>0.3421</v>
+      </c>
+      <c r="E1380">
+        <v>0.3446</v>
+      </c>
+      <c r="F1380">
+        <v>1348635.6</v>
+      </c>
+    </row>
+    <row r="1381" spans="1:6">
+      <c r="A1381" s="2">
+        <v>45536.33333333334</v>
+      </c>
+      <c r="B1381">
+        <v>0.3446</v>
+      </c>
+      <c r="C1381">
+        <v>0.3449</v>
+      </c>
+      <c r="D1381">
+        <v>0.3429</v>
+      </c>
+      <c r="E1381">
+        <v>0.3436</v>
+      </c>
+      <c r="F1381">
+        <v>889862.6</v>
+      </c>
+    </row>
+    <row r="1382" spans="1:6">
+      <c r="A1382" s="2">
+        <v>45536.375</v>
+      </c>
+      <c r="B1382">
+        <v>0.3436</v>
+      </c>
+      <c r="C1382">
+        <v>0.345</v>
+      </c>
+      <c r="D1382">
+        <v>0.343</v>
+      </c>
+      <c r="E1382">
+        <v>0.3439</v>
+      </c>
+      <c r="F1382">
+        <v>672229.6</v>
+      </c>
+    </row>
+    <row r="1383" spans="1:6">
+      <c r="A1383" s="2">
+        <v>45536.41666666666</v>
+      </c>
+      <c r="B1383">
+        <v>0.3439</v>
+      </c>
+      <c r="C1383">
+        <v>0.344</v>
+      </c>
+      <c r="D1383">
+        <v>0.3428</v>
+      </c>
+      <c r="E1383">
+        <v>0.3428</v>
+      </c>
+      <c r="F1383">
+        <v>210265.5</v>
+      </c>
+    </row>
+    <row r="1384" spans="1:6">
+      <c r="A1384" s="2">
+        <v>45536.45833333334</v>
+      </c>
+      <c r="B1384">
+        <v>0.3405</v>
+      </c>
+      <c r="C1384">
+        <v>0.3432</v>
+      </c>
+      <c r="D1384">
+        <v>0.3403</v>
+      </c>
+      <c r="E1384">
+        <v>0.3432</v>
+      </c>
+      <c r="F1384">
+        <v>1719958.5</v>
+      </c>
+    </row>
+    <row r="1385" spans="1:6">
+      <c r="A1385" s="2">
+        <v>45536.5</v>
+      </c>
+      <c r="B1385">
+        <v>0.3431</v>
+      </c>
+      <c r="C1385">
+        <v>0.3436</v>
+      </c>
+      <c r="D1385">
+        <v>0.3386</v>
+      </c>
+      <c r="E1385">
+        <v>0.3392</v>
+      </c>
+      <c r="F1385">
+        <v>2480792.8</v>
+      </c>
+    </row>
+    <row r="1386" spans="1:6">
+      <c r="A1386" s="2">
+        <v>45536.54166666666</v>
+      </c>
+      <c r="B1386">
+        <v>0.3393</v>
+      </c>
+      <c r="C1386">
+        <v>0.341</v>
+      </c>
+      <c r="D1386">
+        <v>0.3363</v>
+      </c>
+      <c r="E1386">
+        <v>0.3405</v>
+      </c>
+      <c r="F1386">
+        <v>4347530.5</v>
+      </c>
+    </row>
+    <row r="1387" spans="1:6">
+      <c r="A1387" s="2">
+        <v>45536.58333333334</v>
+      </c>
+      <c r="B1387">
+        <v>0.3406</v>
+      </c>
+      <c r="C1387">
+        <v>0.3406</v>
+      </c>
+      <c r="D1387">
+        <v>0.3351</v>
+      </c>
+      <c r="E1387">
+        <v>0.3383</v>
+      </c>
+      <c r="F1387">
+        <v>6324687.7</v>
+      </c>
+    </row>
+    <row r="1388" spans="1:6">
+      <c r="A1388" s="2">
+        <v>45536.625</v>
+      </c>
+      <c r="B1388">
+        <v>0.3383</v>
+      </c>
+      <c r="C1388">
+        <v>0.3416</v>
+      </c>
+      <c r="D1388">
+        <v>0.3367</v>
+      </c>
+      <c r="E1388">
+        <v>0.3403</v>
+      </c>
+      <c r="F1388">
+        <v>2607872.4</v>
+      </c>
+    </row>
+    <row r="1389" spans="1:6">
+      <c r="A1389" s="2">
+        <v>45536.66666666666</v>
+      </c>
+      <c r="B1389">
+        <v>0.3403</v>
+      </c>
+      <c r="C1389">
+        <v>0.3417</v>
+      </c>
+      <c r="D1389">
+        <v>0.3378</v>
+      </c>
+      <c r="E1389">
+        <v>0.3384</v>
+      </c>
+      <c r="F1389">
+        <v>2040174.4</v>
+      </c>
+    </row>
+    <row r="1390" spans="1:6">
+      <c r="A1390" s="2">
+        <v>45536.70833333334</v>
+      </c>
+      <c r="B1390">
+        <v>0.3384</v>
+      </c>
+      <c r="C1390">
+        <v>0.3394</v>
+      </c>
+      <c r="D1390">
+        <v>0.3341</v>
+      </c>
+      <c r="E1390">
+        <v>0.3348</v>
+      </c>
+      <c r="F1390">
+        <v>5179954.7</v>
+      </c>
+    </row>
+    <row r="1391" spans="1:6">
+      <c r="A1391" s="2">
+        <v>45536.75</v>
+      </c>
+      <c r="B1391">
+        <v>0.3349</v>
+      </c>
+      <c r="C1391">
+        <v>0.3407</v>
+      </c>
+      <c r="D1391">
+        <v>0.3347</v>
+      </c>
+      <c r="E1391">
+        <v>0.3398</v>
+      </c>
+      <c r="F1391">
+        <v>3508288.6</v>
+      </c>
+    </row>
+    <row r="1392" spans="1:6">
+      <c r="A1392" s="2">
+        <v>45536.79166666666</v>
+      </c>
+      <c r="B1392">
+        <v>0.3398</v>
+      </c>
+      <c r="C1392">
+        <v>0.3422</v>
+      </c>
+      <c r="D1392">
+        <v>0.3391</v>
+      </c>
+      <c r="E1392">
+        <v>0.3397</v>
+      </c>
+      <c r="F1392">
+        <v>2966469</v>
+      </c>
+    </row>
+    <row r="1393" spans="1:6">
+      <c r="A1393" s="2">
+        <v>45536.83333333334</v>
+      </c>
+      <c r="B1393">
+        <v>0.3397</v>
+      </c>
+      <c r="C1393">
+        <v>0.3421</v>
+      </c>
+      <c r="D1393">
+        <v>0.339</v>
+      </c>
+      <c r="E1393">
+        <v>0.3394</v>
+      </c>
+      <c r="F1393">
+        <v>1536658.8</v>
+      </c>
+    </row>
+    <row r="1394" spans="1:6">
+      <c r="A1394" s="2">
+        <v>45536.875</v>
+      </c>
+      <c r="B1394">
+        <v>0.3393</v>
+      </c>
+      <c r="C1394">
+        <v>0.3394</v>
+      </c>
+      <c r="D1394">
+        <v>0.3357</v>
+      </c>
+      <c r="E1394">
+        <v>0.3373</v>
+      </c>
+      <c r="F1394">
+        <v>1695155.9</v>
+      </c>
+    </row>
+    <row r="1395" spans="1:6">
+      <c r="A1395" s="2">
+        <v>45536.91666666666</v>
+      </c>
+      <c r="B1395">
+        <v>0.3374</v>
+      </c>
+      <c r="C1395">
+        <v>0.3378</v>
+      </c>
+      <c r="D1395">
+        <v>0.3267</v>
+      </c>
+      <c r="E1395">
+        <v>0.3284</v>
+      </c>
+      <c r="F1395">
+        <v>10238749.4</v>
+      </c>
+    </row>
+    <row r="1396" spans="1:6">
+      <c r="A1396" s="2">
+        <v>45536.95833333334</v>
+      </c>
+      <c r="B1396">
+        <v>0.3284</v>
+      </c>
+      <c r="C1396">
+        <v>0.3327</v>
+      </c>
+      <c r="D1396">
+        <v>0.3279</v>
+      </c>
+      <c r="E1396">
+        <v>0.3311</v>
+      </c>
+      <c r="F1396">
+        <v>3919326.9</v>
+      </c>
+    </row>
+    <row r="1397" spans="1:6">
+      <c r="A1397" s="2">
+        <v>45537</v>
+      </c>
+      <c r="B1397">
+        <v>0.331</v>
+      </c>
+      <c r="C1397">
+        <v>0.3341</v>
+      </c>
+      <c r="D1397">
+        <v>0.3308</v>
+      </c>
+      <c r="E1397">
+        <v>0.3332</v>
+      </c>
+      <c r="F1397">
+        <v>2228852.5</v>
+      </c>
+    </row>
+    <row r="1398" spans="1:6">
+      <c r="A1398" s="2">
+        <v>45537.04166666666</v>
+      </c>
+      <c r="B1398">
+        <v>0.3332</v>
+      </c>
+      <c r="C1398">
+        <v>0.3345</v>
+      </c>
+      <c r="D1398">
+        <v>0.332</v>
+      </c>
+      <c r="E1398">
+        <v>0.3331</v>
+      </c>
+      <c r="F1398">
+        <v>1525910.7</v>
+      </c>
+    </row>
+    <row r="1399" spans="1:6">
+      <c r="A1399" s="2">
+        <v>45537.08333333334</v>
+      </c>
+      <c r="B1399">
+        <v>0.3332</v>
+      </c>
+      <c r="C1399">
+        <v>0.3345</v>
+      </c>
+      <c r="D1399">
+        <v>0.3314</v>
+      </c>
+      <c r="E1399">
+        <v>0.3326</v>
+      </c>
+      <c r="F1399">
+        <v>1731650.3</v>
+      </c>
+    </row>
+    <row r="1400" spans="1:6">
+      <c r="A1400" s="2">
+        <v>45537.125</v>
+      </c>
+      <c r="B1400">
+        <v>0.3326</v>
+      </c>
+      <c r="C1400">
+        <v>0.3339</v>
+      </c>
+      <c r="D1400">
+        <v>0.331</v>
+      </c>
+      <c r="E1400">
+        <v>0.3316</v>
+      </c>
+      <c r="F1400">
+        <v>1154532.1</v>
+      </c>
+    </row>
+    <row r="1401" spans="1:6">
+      <c r="A1401" s="2">
+        <v>45537.16666666666</v>
+      </c>
+      <c r="B1401">
+        <v>0.3315</v>
+      </c>
+      <c r="C1401">
+        <v>0.3316</v>
+      </c>
+      <c r="D1401">
+        <v>0.3271</v>
+      </c>
+      <c r="E1401">
+        <v>0.3272</v>
+      </c>
+      <c r="F1401">
+        <v>2173622.9</v>
+      </c>
+    </row>
+    <row r="1402" spans="1:6">
+      <c r="A1402" s="2">
+        <v>45537.20833333334</v>
+      </c>
+      <c r="B1402">
+        <v>0.3272</v>
+      </c>
+      <c r="C1402">
+        <v>0.3315</v>
+      </c>
+      <c r="D1402">
+        <v>0.3271</v>
+      </c>
+      <c r="E1402">
+        <v>0.3301</v>
+      </c>
+      <c r="F1402">
+        <v>3237801</v>
+      </c>
+    </row>
+    <row r="1403" spans="1:6">
+      <c r="A1403" s="2">
+        <v>45537.25</v>
+      </c>
+      <c r="B1403">
+        <v>0.3301</v>
+      </c>
+      <c r="C1403">
+        <v>0.3312</v>
+      </c>
+      <c r="D1403">
+        <v>0.3289</v>
+      </c>
+      <c r="E1403">
+        <v>0.3305</v>
+      </c>
+      <c r="F1403">
+        <v>1871660.7</v>
+      </c>
+    </row>
+    <row r="1404" spans="1:6">
+      <c r="A1404" s="2">
+        <v>45537.29166666666</v>
+      </c>
+      <c r="B1404">
+        <v>0.3305</v>
+      </c>
+      <c r="C1404">
+        <v>0.3305</v>
+      </c>
+      <c r="D1404">
+        <v>0.325</v>
+      </c>
+      <c r="E1404">
+        <v>0.3259</v>
+      </c>
+      <c r="F1404">
+        <v>4031985</v>
+      </c>
+    </row>
+    <row r="1405" spans="1:6">
+      <c r="A1405" s="2">
+        <v>45537.33333333334</v>
+      </c>
+      <c r="B1405">
+        <v>0.3259</v>
+      </c>
+      <c r="C1405">
+        <v>0.3321</v>
+      </c>
+      <c r="D1405">
+        <v>0.3253</v>
+      </c>
+      <c r="E1405">
+        <v>0.3297</v>
+      </c>
+      <c r="F1405">
+        <v>5349799.5</v>
+      </c>
+    </row>
+    <row r="1406" spans="1:6">
+      <c r="A1406" s="2">
+        <v>45537.375</v>
+      </c>
+      <c r="B1406">
+        <v>0.3296</v>
+      </c>
+      <c r="C1406">
+        <v>0.3327</v>
+      </c>
+      <c r="D1406">
+        <v>0.3262</v>
+      </c>
+      <c r="E1406">
+        <v>0.3322</v>
+      </c>
+      <c r="F1406">
+        <v>8474220</v>
+      </c>
+    </row>
+    <row r="1407" spans="1:6">
+      <c r="A1407" s="2">
+        <v>45537.41666666666</v>
+      </c>
+      <c r="B1407">
+        <v>0.3322</v>
+      </c>
+      <c r="C1407">
+        <v>0.3349</v>
+      </c>
+      <c r="D1407">
+        <v>0.3314</v>
+      </c>
+      <c r="E1407">
+        <v>0.334</v>
+      </c>
+      <c r="F1407">
+        <v>3349446.2</v>
+      </c>
+    </row>
+    <row r="1408" spans="1:6">
+      <c r="A1408" s="2">
+        <v>45537.45833333334</v>
+      </c>
+      <c r="B1408">
+        <v>0.3339</v>
+      </c>
+      <c r="C1408">
+        <v>0.3364</v>
+      </c>
+      <c r="D1408">
+        <v>0.3331</v>
+      </c>
+      <c r="E1408">
+        <v>0.3346</v>
+      </c>
+      <c r="F1408">
+        <v>2356133.8</v>
+      </c>
+    </row>
+    <row r="1409" spans="1:6">
+      <c r="A1409" s="2">
+        <v>45537.5</v>
+      </c>
+      <c r="B1409">
+        <v>0.3338</v>
+      </c>
+      <c r="C1409">
+        <v>0.3349</v>
+      </c>
+      <c r="D1409">
+        <v>0.3313</v>
+      </c>
+      <c r="E1409">
+        <v>0.3324</v>
+      </c>
+      <c r="F1409">
+        <v>3058725</v>
+      </c>
+    </row>
+    <row r="1410" spans="1:6">
+      <c r="A1410" s="2">
+        <v>45537.54166666666</v>
+      </c>
+      <c r="B1410">
+        <v>0.3323</v>
+      </c>
+      <c r="C1410">
+        <v>0.3328</v>
+      </c>
+      <c r="D1410">
+        <v>0.3287</v>
+      </c>
+      <c r="E1410">
+        <v>0.3287</v>
+      </c>
+      <c r="F1410">
+        <v>2424780.8</v>
+      </c>
+    </row>
+    <row r="1411" spans="1:6">
+      <c r="A1411" s="2">
+        <v>45537.58333333334</v>
+      </c>
+      <c r="B1411">
+        <v>0.3287</v>
+      </c>
+      <c r="C1411">
+        <v>0.3335</v>
+      </c>
+      <c r="D1411">
+        <v>0.3269</v>
+      </c>
+      <c r="E1411">
+        <v>0.3331</v>
+      </c>
+      <c r="F1411">
+        <v>7238348.6</v>
+      </c>
+    </row>
+    <row r="1412" spans="1:6">
+      <c r="A1412" s="2">
+        <v>45537.625</v>
+      </c>
+      <c r="B1412">
+        <v>0.333</v>
+      </c>
+      <c r="C1412">
+        <v>0.3339</v>
+      </c>
+      <c r="D1412">
+        <v>0.3315</v>
+      </c>
+      <c r="E1412">
+        <v>0.3325</v>
+      </c>
+      <c r="F1412">
+        <v>2665624</v>
+      </c>
+    </row>
+    <row r="1413" spans="1:6">
+      <c r="A1413" s="2">
+        <v>45537.66666666666</v>
+      </c>
+      <c r="B1413">
+        <v>0.3325</v>
+      </c>
+      <c r="C1413">
+        <v>0.3342</v>
+      </c>
+      <c r="D1413">
+        <v>0.3297</v>
+      </c>
+      <c r="E1413">
+        <v>0.3298</v>
+      </c>
+      <c r="F1413">
+        <v>1885936.3</v>
+      </c>
+    </row>
+    <row r="1414" spans="1:6">
+      <c r="A1414" s="2">
+        <v>45537.70833333334</v>
+      </c>
+      <c r="B1414">
+        <v>0.3298</v>
+      </c>
+      <c r="C1414">
+        <v>0.3337</v>
+      </c>
+      <c r="D1414">
+        <v>0.3297</v>
+      </c>
+      <c r="E1414">
+        <v>0.3332</v>
+      </c>
+      <c r="F1414">
+        <v>1532810.1</v>
+      </c>
+    </row>
+    <row r="1415" spans="1:6">
+      <c r="A1415" s="2">
+        <v>45537.75</v>
+      </c>
+      <c r="B1415">
+        <v>0.3333</v>
+      </c>
+      <c r="C1415">
+        <v>0.3335</v>
+      </c>
+      <c r="D1415">
+        <v>0.3298</v>
+      </c>
+      <c r="E1415">
+        <v>0.3312</v>
+      </c>
+      <c r="F1415">
+        <v>3237909.5</v>
+      </c>
+    </row>
+    <row r="1416" spans="1:6">
+      <c r="A1416" s="2">
+        <v>45537.79166666666</v>
+      </c>
+      <c r="B1416">
+        <v>0.3312</v>
+      </c>
+      <c r="C1416">
+        <v>0.3325</v>
+      </c>
+      <c r="D1416">
+        <v>0.3302</v>
+      </c>
+      <c r="E1416">
+        <v>0.3309</v>
+      </c>
+      <c r="F1416">
+        <v>2650201.9</v>
+      </c>
+    </row>
+    <row r="1417" spans="1:6">
+      <c r="A1417" s="2">
+        <v>45537.83333333334</v>
+      </c>
+      <c r="B1417">
+        <v>0.3309</v>
+      </c>
+      <c r="C1417">
+        <v>0.337</v>
+      </c>
+      <c r="D1417">
+        <v>0.3303</v>
+      </c>
+      <c r="E1417">
+        <v>0.3355</v>
+      </c>
+      <c r="F1417">
+        <v>2203585.1</v>
+      </c>
+    </row>
+    <row r="1418" spans="1:6">
+      <c r="A1418" s="2">
+        <v>45537.875</v>
+      </c>
+      <c r="B1418">
+        <v>0.3355</v>
+      </c>
+      <c r="C1418">
+        <v>0.3374</v>
+      </c>
+      <c r="D1418">
+        <v>0.3353</v>
+      </c>
+      <c r="E1418">
+        <v>0.3364</v>
+      </c>
+      <c r="F1418">
+        <v>2234022</v>
+      </c>
+    </row>
+    <row r="1419" spans="1:6">
+      <c r="A1419" s="2">
+        <v>45537.91666666666</v>
+      </c>
+      <c r="B1419">
+        <v>0.3364</v>
+      </c>
+      <c r="C1419">
+        <v>0.337</v>
+      </c>
+      <c r="D1419">
+        <v>0.3347</v>
+      </c>
+      <c r="E1419">
+        <v>0.3364</v>
+      </c>
+      <c r="F1419">
+        <v>1888980.8</v>
+      </c>
+    </row>
+    <row r="1420" spans="1:6">
+      <c r="A1420" s="2">
+        <v>45537.95833333334</v>
+      </c>
+      <c r="B1420">
+        <v>0.3363</v>
+      </c>
+      <c r="C1420">
+        <v>0.337</v>
+      </c>
+      <c r="D1420">
+        <v>0.3353</v>
+      </c>
+      <c r="E1420">
+        <v>0.3362</v>
+      </c>
+      <c r="F1420">
+        <v>1683704.2</v>
+      </c>
+    </row>
+    <row r="1421" spans="1:6">
+      <c r="A1421" s="2">
+        <v>45538</v>
+      </c>
+      <c r="B1421">
+        <v>0.3362</v>
+      </c>
+      <c r="C1421">
+        <v>0.3365</v>
+      </c>
+      <c r="D1421">
+        <v>0.3346</v>
+      </c>
+      <c r="E1421">
+        <v>0.3357</v>
+      </c>
+      <c r="F1421">
+        <v>3129415.4</v>
+      </c>
+    </row>
+    <row r="1422" spans="1:6">
+      <c r="A1422" s="2">
+        <v>45538.04166666666</v>
+      </c>
+      <c r="B1422">
+        <v>0.3356</v>
+      </c>
+      <c r="C1422">
+        <v>0.337</v>
+      </c>
+      <c r="D1422">
+        <v>0.3342</v>
+      </c>
+      <c r="E1422">
+        <v>0.3361</v>
+      </c>
+      <c r="F1422">
+        <v>1768109</v>
+      </c>
+    </row>
+    <row r="1423" spans="1:6">
+      <c r="A1423" s="2">
+        <v>45538.08333333334</v>
+      </c>
+      <c r="B1423">
+        <v>0.336</v>
+      </c>
+      <c r="C1423">
+        <v>0.3398</v>
+      </c>
+      <c r="D1423">
+        <v>0.3356</v>
+      </c>
+      <c r="E1423">
+        <v>0.3364</v>
+      </c>
+      <c r="F1423">
+        <v>3624195.9</v>
+      </c>
+    </row>
+    <row r="1424" spans="1:6">
+      <c r="A1424" s="2">
+        <v>45538.125</v>
+      </c>
+      <c r="B1424">
+        <v>0.3364</v>
+      </c>
+      <c r="C1424">
+        <v>0.3366</v>
+      </c>
+      <c r="D1424">
+        <v>0.3348</v>
+      </c>
+      <c r="E1424">
+        <v>0.3351</v>
+      </c>
+      <c r="F1424">
+        <v>1479711</v>
+      </c>
+    </row>
+    <row r="1425" spans="1:6">
+      <c r="A1425" s="2">
+        <v>45538.16666666666</v>
+      </c>
+      <c r="B1425">
+        <v>0.3352</v>
+      </c>
+      <c r="C1425">
+        <v>0.3356</v>
+      </c>
+      <c r="D1425">
+        <v>0.3334</v>
+      </c>
+      <c r="E1425">
+        <v>0.3338</v>
+      </c>
+      <c r="F1425">
+        <v>1993514.7</v>
+      </c>
+    </row>
+    <row r="1426" spans="1:6">
+      <c r="A1426" s="2">
+        <v>45538.20833333334</v>
+      </c>
+      <c r="B1426">
+        <v>0.3339</v>
+      </c>
+      <c r="C1426">
+        <v>0.3345</v>
+      </c>
+      <c r="D1426">
+        <v>0.3329</v>
+      </c>
+      <c r="E1426">
+        <v>0.3341</v>
+      </c>
+      <c r="F1426">
+        <v>1230247.2</v>
+      </c>
+    </row>
+    <row r="1427" spans="1:6">
+      <c r="A1427" s="2">
+        <v>45538.25</v>
+      </c>
+      <c r="B1427">
+        <v>0.3341</v>
+      </c>
+      <c r="C1427">
+        <v>0.3341</v>
+      </c>
+      <c r="D1427">
+        <v>0.3319</v>
+      </c>
+      <c r="E1427">
+        <v>0.332</v>
+      </c>
+      <c r="F1427">
+        <v>1803616</v>
+      </c>
+    </row>
+    <row r="1428" spans="1:6">
+      <c r="A1428" s="2">
+        <v>45538.29166666666</v>
+      </c>
+      <c r="B1428">
+        <v>0.332</v>
+      </c>
+      <c r="C1428">
+        <v>0.3337</v>
+      </c>
+      <c r="D1428">
+        <v>0.3318</v>
+      </c>
+      <c r="E1428">
+        <v>0.3334</v>
+      </c>
+      <c r="F1428">
+        <v>1983998.8</v>
+      </c>
+    </row>
+    <row r="1429" spans="1:6">
+      <c r="A1429" s="2">
+        <v>45538.33333333334</v>
+      </c>
+      <c r="B1429">
+        <v>0.3335</v>
+      </c>
+      <c r="C1429">
+        <v>0.3336</v>
+      </c>
+      <c r="D1429">
+        <v>0.3282</v>
+      </c>
+      <c r="E1429">
+        <v>0.3286</v>
+      </c>
+      <c r="F1429">
+        <v>4373229.8</v>
+      </c>
+    </row>
+    <row r="1430" spans="1:6">
+      <c r="A1430" s="2">
+        <v>45538.375</v>
+      </c>
+      <c r="B1430">
+        <v>0.3285</v>
+      </c>
+      <c r="C1430">
+        <v>0.3297</v>
+      </c>
+      <c r="D1430">
+        <v>0.3281</v>
+      </c>
+      <c r="E1430">
+        <v>0.3291</v>
+      </c>
+      <c r="F1430">
+        <v>2291833.7</v>
+      </c>
+    </row>
+    <row r="1431" spans="1:6">
+      <c r="A1431" s="2">
+        <v>45538.41666666666</v>
+      </c>
+      <c r="B1431">
+        <v>0.329</v>
+      </c>
+      <c r="C1431">
+        <v>0.3312</v>
+      </c>
+      <c r="D1431">
+        <v>0.3286</v>
+      </c>
+      <c r="E1431">
+        <v>0.3302</v>
+      </c>
+      <c r="F1431">
+        <v>2165979.2</v>
+      </c>
+    </row>
+    <row r="1432" spans="1:6">
+      <c r="A1432" s="2">
+        <v>45538.45833333334</v>
+      </c>
+      <c r="B1432">
+        <v>0.3302</v>
+      </c>
+      <c r="C1432">
+        <v>0.3308</v>
+      </c>
+      <c r="D1432">
+        <v>0.3292</v>
+      </c>
+      <c r="E1432">
+        <v>0.3302</v>
+      </c>
+      <c r="F1432">
+        <v>1529538.8</v>
+      </c>
+    </row>
+    <row r="1433" spans="1:6">
+      <c r="A1433" s="2">
+        <v>45538.5</v>
+      </c>
+      <c r="B1433">
+        <v>0.3302</v>
+      </c>
+      <c r="C1433">
+        <v>0.332</v>
+      </c>
+      <c r="D1433">
+        <v>0.3299</v>
+      </c>
+      <c r="E1433">
+        <v>0.3301</v>
+      </c>
+      <c r="F1433">
+        <v>2236298.8</v>
+      </c>
+    </row>
+    <row r="1434" spans="1:6">
+      <c r="A1434" s="2">
+        <v>45538.54166666666</v>
+      </c>
+      <c r="B1434">
+        <v>0.3301</v>
+      </c>
+      <c r="C1434">
+        <v>0.3315</v>
+      </c>
+      <c r="D1434">
+        <v>0.3227</v>
+      </c>
+      <c r="E1434">
+        <v>0.3243</v>
+      </c>
+      <c r="F1434">
+        <v>10111634.9</v>
+      </c>
+    </row>
+    <row r="1435" spans="1:6">
+      <c r="A1435" s="2">
+        <v>45538.58333333334</v>
+      </c>
+      <c r="B1435">
+        <v>0.3242</v>
+      </c>
+      <c r="C1435">
+        <v>0.3242</v>
+      </c>
+      <c r="D1435">
+        <v>0.3201</v>
+      </c>
+      <c r="E1435">
+        <v>0.3216</v>
+      </c>
+      <c r="F1435">
+        <v>9480525.9</v>
+      </c>
+    </row>
+    <row r="1436" spans="1:6">
+      <c r="A1436" s="2">
+        <v>45538.625</v>
+      </c>
+      <c r="B1436">
+        <v>0.3216</v>
+      </c>
+      <c r="C1436">
+        <v>0.3227</v>
+      </c>
+      <c r="D1436">
+        <v>0.32</v>
+      </c>
+      <c r="E1436">
+        <v>0.3204</v>
+      </c>
+      <c r="F1436">
+        <v>5119799.6</v>
+      </c>
+    </row>
+    <row r="1437" spans="1:6">
+      <c r="A1437" s="2">
+        <v>45538.66666666666</v>
+      </c>
+      <c r="B1437">
+        <v>0.3204</v>
+      </c>
+      <c r="C1437">
+        <v>0.3225</v>
+      </c>
+      <c r="D1437">
+        <v>0.3195</v>
+      </c>
+      <c r="E1437">
+        <v>0.3217</v>
+      </c>
+      <c r="F1437">
+        <v>3120274.9</v>
+      </c>
+    </row>
+    <row r="1438" spans="1:6">
+      <c r="A1438" s="2">
+        <v>45538.70833333334</v>
+      </c>
+      <c r="B1438">
+        <v>0.3216</v>
+      </c>
+      <c r="C1438">
+        <v>0.3253</v>
+      </c>
+      <c r="D1438">
+        <v>0.3215</v>
+      </c>
+      <c r="E1438">
+        <v>0.3233</v>
+      </c>
+      <c r="F1438">
+        <v>2545136</v>
+      </c>
+    </row>
+    <row r="1439" spans="1:6">
+      <c r="A1439" s="2">
+        <v>45538.75</v>
+      </c>
+      <c r="B1439">
+        <v>0.3233</v>
+      </c>
+      <c r="C1439">
+        <v>0.3244</v>
+      </c>
+      <c r="D1439">
+        <v>0.3221</v>
+      </c>
+      <c r="E1439">
+        <v>0.3236</v>
+      </c>
+      <c r="F1439">
+        <v>1929059.4</v>
+      </c>
+    </row>
+    <row r="1440" spans="1:6">
+      <c r="A1440" s="2">
+        <v>45538.79166666666</v>
+      </c>
+      <c r="B1440">
+        <v>0.3236</v>
+      </c>
+      <c r="C1440">
+        <v>0.3259</v>
+      </c>
+      <c r="D1440">
+        <v>0.3225</v>
+      </c>
+      <c r="E1440">
+        <v>0.3249</v>
+      </c>
+      <c r="F1440">
+        <v>1884666.6</v>
+      </c>
+    </row>
+    <row r="1441" spans="1:6">
+      <c r="A1441" s="2">
+        <v>45538.83333333334</v>
+      </c>
+      <c r="B1441">
+        <v>0.3249</v>
+      </c>
+      <c r="C1441">
+        <v>0.3262</v>
+      </c>
+      <c r="D1441">
+        <v>0.3238</v>
+      </c>
+      <c r="E1441">
+        <v>0.3247</v>
+      </c>
+      <c r="F1441">
+        <v>1358022.4</v>
+      </c>
+    </row>
+    <row r="1442" spans="1:6">
+      <c r="A1442" s="2">
+        <v>45538.875</v>
+      </c>
+      <c r="B1442">
+        <v>0.3248</v>
+      </c>
+      <c r="C1442">
+        <v>0.3248</v>
+      </c>
+      <c r="D1442">
+        <v>0.3222</v>
+      </c>
+      <c r="E1442">
+        <v>0.3231</v>
+      </c>
+      <c r="F1442">
+        <v>1622509.3</v>
+      </c>
+    </row>
+    <row r="1443" spans="1:6">
+      <c r="A1443" s="2">
+        <v>45538.91666666666</v>
+      </c>
+      <c r="B1443">
+        <v>0.3231</v>
+      </c>
+      <c r="C1443">
+        <v>0.3236</v>
+      </c>
+      <c r="D1443">
+        <v>0.3208</v>
+      </c>
+      <c r="E1443">
+        <v>0.3208</v>
+      </c>
+      <c r="F1443">
+        <v>1655313.4</v>
+      </c>
+    </row>
+    <row r="1444" spans="1:6">
+      <c r="A1444" s="2">
+        <v>45538.95833333334</v>
+      </c>
+      <c r="B1444">
+        <v>0.3209</v>
+      </c>
+      <c r="C1444">
+        <v>0.3212</v>
+      </c>
+      <c r="D1444">
+        <v>0.3172</v>
+      </c>
+      <c r="E1444">
+        <v>0.3185</v>
+      </c>
+      <c r="F1444">
+        <v>7038114.7</v>
+      </c>
+    </row>
+    <row r="1445" spans="1:6">
+      <c r="A1445" s="2">
+        <v>45539</v>
+      </c>
+      <c r="B1445">
+        <v>0.3184</v>
+      </c>
+      <c r="C1445">
+        <v>0.3202</v>
+      </c>
+      <c r="D1445">
+        <v>0.3149</v>
+      </c>
+      <c r="E1445">
+        <v>0.3157</v>
+      </c>
+      <c r="F1445">
+        <v>6372050.6</v>
+      </c>
+    </row>
+    <row r="1446" spans="1:6">
+      <c r="A1446" s="2">
+        <v>45539.04166666666</v>
+      </c>
+      <c r="B1446">
+        <v>0.3158</v>
+      </c>
+      <c r="C1446">
+        <v>0.3159</v>
+      </c>
+      <c r="D1446">
+        <v>0.305</v>
+      </c>
+      <c r="E1446">
+        <v>0.3143</v>
+      </c>
+      <c r="F1446">
+        <v>28089872.8</v>
+      </c>
+    </row>
+    <row r="1447" spans="1:6">
+      <c r="A1447" s="2">
+        <v>45539.08333333334</v>
+      </c>
+      <c r="B1447">
+        <v>0.3143</v>
+      </c>
+      <c r="C1447">
+        <v>0.3167</v>
+      </c>
+      <c r="D1447">
+        <v>0.3135</v>
+      </c>
+      <c r="E1447">
+        <v>0.3143</v>
+      </c>
+      <c r="F1447">
+        <v>3983006.6</v>
+      </c>
+    </row>
+    <row r="1448" spans="1:6">
+      <c r="A1448" s="2">
+        <v>45539.125</v>
+      </c>
+      <c r="B1448">
+        <v>0.3144</v>
+      </c>
+      <c r="C1448">
+        <v>0.317</v>
+      </c>
+      <c r="D1448">
+        <v>0.3137</v>
+      </c>
+      <c r="E1448">
+        <v>0.3157</v>
+      </c>
+      <c r="F1448">
+        <v>6337143.1</v>
+      </c>
+    </row>
+    <row r="1449" spans="1:6">
+      <c r="A1449" s="2">
+        <v>45539.16666666666</v>
+      </c>
+      <c r="B1449">
+        <v>0.3157</v>
+      </c>
+      <c r="C1449">
+        <v>0.3172</v>
+      </c>
+      <c r="D1449">
+        <v>0.3157</v>
+      </c>
+      <c r="E1449">
+        <v>0.3167</v>
+      </c>
+      <c r="F1449">
+        <v>2546665.7</v>
+      </c>
+    </row>
+    <row r="1450" spans="1:6">
+      <c r="A1450" s="2">
+        <v>45539.20833333334</v>
+      </c>
+      <c r="B1450">
+        <v>0.3166</v>
+      </c>
+      <c r="C1450">
+        <v>0.3166</v>
+      </c>
+      <c r="D1450">
+        <v>0.3124</v>
+      </c>
+      <c r="E1450">
+        <v>0.313</v>
+      </c>
+      <c r="F1450">
+        <v>3517048.3</v>
+      </c>
+    </row>
+    <row r="1451" spans="1:6">
+      <c r="A1451" s="2">
+        <v>45539.25</v>
+      </c>
+      <c r="B1451">
+        <v>0.313</v>
+      </c>
+      <c r="C1451">
+        <v>0.3165</v>
+      </c>
+      <c r="D1451">
+        <v>0.313</v>
+      </c>
+      <c r="E1451">
+        <v>0.3148</v>
+      </c>
+      <c r="F1451">
+        <v>3221283.6</v>
+      </c>
+    </row>
+    <row r="1452" spans="1:6">
+      <c r="A1452" s="2">
+        <v>45539.29166666666</v>
+      </c>
+      <c r="B1452">
+        <v>0.3148</v>
+      </c>
+      <c r="C1452">
+        <v>0.3222</v>
+      </c>
+      <c r="D1452">
+        <v>0.3146</v>
+      </c>
+      <c r="E1452">
+        <v>0.3212</v>
+      </c>
+      <c r="F1452">
+        <v>7279927.1</v>
+      </c>
+    </row>
+    <row r="1453" spans="1:6">
+      <c r="A1453" s="2">
+        <v>45539.33333333334</v>
+      </c>
+      <c r="B1453">
+        <v>0.3212</v>
+      </c>
+      <c r="C1453">
+        <v>0.3237</v>
+      </c>
+      <c r="D1453">
+        <v>0.321</v>
+      </c>
+      <c r="E1453">
+        <v>0.3235</v>
+      </c>
+      <c r="F1453">
+        <v>2740497.3</v>
+      </c>
+    </row>
+    <row r="1454" spans="1:6">
+      <c r="A1454" s="2">
+        <v>45539.375</v>
+      </c>
+      <c r="B1454">
+        <v>0.3234</v>
+      </c>
+      <c r="C1454">
+        <v>0.325</v>
+      </c>
+      <c r="D1454">
+        <v>0.3218</v>
+      </c>
+      <c r="E1454">
+        <v>0.3218</v>
+      </c>
+      <c r="F1454">
+        <v>3708488.2</v>
+      </c>
+    </row>
+    <row r="1455" spans="1:6">
+      <c r="A1455" s="2">
+        <v>45539.41666666666</v>
+      </c>
+      <c r="B1455">
+        <v>0.3218</v>
+      </c>
+      <c r="C1455">
+        <v>0.322</v>
+      </c>
+      <c r="D1455">
+        <v>0.318</v>
+      </c>
+      <c r="E1455">
+        <v>0.3182</v>
+      </c>
+      <c r="F1455">
+        <v>3233228.9</v>
+      </c>
+    </row>
+    <row r="1456" spans="1:6">
+      <c r="A1456" s="2">
+        <v>45539.45833333334</v>
+      </c>
+      <c r="B1456">
+        <v>0.3182</v>
+      </c>
+      <c r="C1456">
+        <v>0.3201</v>
+      </c>
+      <c r="D1456">
+        <v>0.315</v>
+      </c>
+      <c r="E1456">
+        <v>0.3175</v>
+      </c>
+      <c r="F1456">
+        <v>7073965.5</v>
+      </c>
+    </row>
+    <row r="1457" spans="1:6">
+      <c r="A1457" s="2">
+        <v>45539.5</v>
+      </c>
+      <c r="B1457">
+        <v>0.3176</v>
+      </c>
+      <c r="C1457">
+        <v>0.3204</v>
+      </c>
+      <c r="D1457">
+        <v>0.3165</v>
+      </c>
+      <c r="E1457">
+        <v>0.3181</v>
+      </c>
+      <c r="F1457">
+        <v>2506937.8</v>
+      </c>
+    </row>
+    <row r="1458" spans="1:6">
+      <c r="A1458" s="2">
+        <v>45539.54166666666</v>
+      </c>
+      <c r="B1458">
+        <v>0.3181</v>
+      </c>
+      <c r="C1458">
+        <v>0.3186</v>
+      </c>
+      <c r="D1458">
+        <v>0.3163</v>
+      </c>
+      <c r="E1458">
+        <v>0.318</v>
+      </c>
+      <c r="F1458">
+        <v>2338156</v>
+      </c>
+    </row>
+    <row r="1459" spans="1:6">
+      <c r="A1459" s="2">
+        <v>45539.58333333334</v>
+      </c>
+      <c r="B1459">
+        <v>0.318</v>
+      </c>
+      <c r="C1459">
+        <v>0.3237</v>
+      </c>
+      <c r="D1459">
+        <v>0.3154</v>
+      </c>
+      <c r="E1459">
+        <v>0.3227</v>
+      </c>
+      <c r="F1459">
+        <v>7139696.9</v>
+      </c>
+    </row>
+    <row r="1460" spans="1:6">
+      <c r="A1460" s="2">
+        <v>45539.625</v>
+      </c>
+      <c r="B1460">
+        <v>0.3228</v>
+      </c>
+      <c r="C1460">
+        <v>0.3262</v>
+      </c>
+      <c r="D1460">
+        <v>0.3222</v>
+      </c>
+      <c r="E1460">
+        <v>0.326</v>
+      </c>
+      <c r="F1460">
+        <v>5403060.5</v>
+      </c>
+    </row>
+    <row r="1461" spans="1:6">
+      <c r="A1461" s="2">
+        <v>45539.66666666666</v>
+      </c>
+      <c r="B1461">
+        <v>0.3259</v>
+      </c>
+      <c r="C1461">
+        <v>0.3293</v>
+      </c>
+      <c r="D1461">
+        <v>0.3255</v>
+      </c>
+      <c r="E1461">
+        <v>0.3263</v>
+      </c>
+      <c r="F1461">
+        <v>6479062.8</v>
+      </c>
+    </row>
+    <row r="1462" spans="1:6">
+      <c r="A1462" s="2">
+        <v>45539.70833333334</v>
+      </c>
+      <c r="B1462">
+        <v>0.3263</v>
+      </c>
+      <c r="C1462">
+        <v>0.3264</v>
+      </c>
+      <c r="D1462">
+        <v>0.3223</v>
+      </c>
+      <c r="E1462">
+        <v>0.3223</v>
+      </c>
+      <c r="F1462">
+        <v>4157784.7</v>
+      </c>
+    </row>
+    <row r="1463" spans="1:6">
+      <c r="A1463" s="2">
+        <v>45539.75</v>
+      </c>
+      <c r="B1463">
+        <v>0.3223</v>
+      </c>
+      <c r="C1463">
+        <v>0.3233</v>
+      </c>
+      <c r="D1463">
+        <v>0.321</v>
+      </c>
+      <c r="E1463">
+        <v>0.3215</v>
+      </c>
+      <c r="F1463">
+        <v>2187408.1</v>
+      </c>
+    </row>
+    <row r="1464" spans="1:6">
+      <c r="A1464" s="2">
+        <v>45539.79166666666</v>
+      </c>
+      <c r="B1464">
+        <v>0.3217</v>
+      </c>
+      <c r="C1464">
+        <v>0.323</v>
+      </c>
+      <c r="D1464">
+        <v>0.3214</v>
+      </c>
+      <c r="E1464">
+        <v>0.3223</v>
+      </c>
+      <c r="F1464">
+        <v>1337768.9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>